<commit_message>
Data read from excel sheet in post request method implemented
</commit_message>
<xml_diff>
--- a/src/main/java/com/eo/util/DataUtil.xlsx
+++ b/src/main/java/com/eo/util/DataUtil.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="65">
   <si>
     <t>Title</t>
   </si>
@@ -239,12 +239,6 @@
     <t>tester</t>
   </si>
   <si>
-    <t>@&amp;^</t>
-  </si>
-  <si>
-    <t>$%*</t>
-  </si>
-  <si>
     <t>Status Code 200 OK. But total number of data objects generated are 6, displayed in response body.</t>
   </si>
   <si>
@@ -252,6 +246,9 @@
   </si>
   <si>
     <t>Status code: 200;                            verify total user count:12</t>
+  </si>
+  <si>
+    <t>Urmila</t>
   </si>
 </sst>
 </file>
@@ -755,7 +752,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:O9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView topLeftCell="G1" workbookViewId="0">
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
@@ -870,16 +867,16 @@
         <v>9</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I4" s="6" t="s">
         <v>38</v>
       </c>
       <c r="J4" s="25" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K4" s="26" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L4" s="18"/>
       <c r="M4" s="18"/>
@@ -1096,8 +1093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1119,19 +1116,19 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="24">
-        <v>123</v>
-      </c>
-      <c r="B3" s="24">
-        <v>456</v>
+      <c r="A3" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="24" t="s">
-        <v>62</v>
+      <c r="A4" s="24">
+        <v>123</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>